<commit_message>
Mise en place du JSON vers le xlsx, je peux désormais faire d'un côté ou de l'autre
</commit_message>
<xml_diff>
--- a/src/ExcelData/ClasseurToImplement.xlsx
+++ b/src/ExcelData/ClasseurToImplement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\luc.chesneau\Documents\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7294635F-7D4B-417D-8C9C-8C51576BC0AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{871BB01F-3644-4B42-BA5E-DC82C9E3628E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F6F82B82-B185-4832-AE1E-D395F1B17350}"/>
   </bookViews>
@@ -454,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D408A1DD-9D40-4EAF-B24E-14E7084C3137}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="A2:D11"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
@@ -479,43 +479,29 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s">
-        <v>19</v>
-      </c>
-    </row>
     <row r="3" spans="1:4">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
         <v>17</v>
@@ -523,13 +509,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
         <v>17</v>
@@ -537,55 +523,55 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
         <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
         <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>19</v>
@@ -593,29 +579,43 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" t="s">
-        <v>17</v>
+        <v>14</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>12</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>14</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D12" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>